<commit_message>
pom.xml updated for compiler error test 1
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -30,28 +30,28 @@
     <t>description</t>
   </si>
   <si>
-    <t>Jane23 White</t>
-  </si>
-  <si>
-    <t>Jane23@way2automation.com</t>
+    <t>Jane26 White</t>
+  </si>
+  <si>
+    <t>Jane26@way2automation.com</t>
   </si>
   <si>
     <t>Adding first customer in framework</t>
   </si>
   <si>
-    <t>Jone23 Fong</t>
-  </si>
-  <si>
-    <t>Jone23@way3automation.com</t>
+    <t>Jone26 Fong</t>
+  </si>
+  <si>
+    <t>Jone26@way3automation.com</t>
   </si>
   <si>
     <t>Adding second customer in framework</t>
   </si>
   <si>
-    <t>Ishita23 Aron</t>
-  </si>
-  <si>
-    <t>Ishita23@way3automation.com</t>
+    <t>Ishita26 Aron</t>
+  </si>
+  <si>
+    <t>Ishita26@way3automation.com</t>
   </si>
   <si>
     <t>Adding third customer in framework</t>
@@ -101,10 +101,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -131,8 +131,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,6 +146,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -152,31 +161,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -230,6 +224,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -238,15 +246,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -268,13 +268,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,169 +430,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,19 +480,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -538,24 +551,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -573,139 +573,139 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -1144,9 +1144,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="Jane23@way2automation.com" tooltip="mailto:Jane23@way2automation.com"/>
-    <hyperlink ref="B4" r:id="rId2" display="Jone23@way3automation.com" tooltip="mailto:Jone23@way3automation.com"/>
-    <hyperlink ref="B5" r:id="rId3" display="Ishita23@way3automation.com" tooltip="mailto:Ishita23@way3automation.com"/>
+    <hyperlink ref="B3" r:id="rId1" display="Jane26@way2automation.com" tooltip="mailto:Jane26@way2automation.com"/>
+    <hyperlink ref="B4" r:id="rId2" display="Jone26@way3automation.com" tooltip="mailto:Jone26@way3automation.com"/>
+    <hyperlink ref="B5" r:id="rId3" display="Ishita26@way3automation.com" tooltip="mailto:Ishita26@way3automation.com"/>
     <hyperlink ref="B9" r:id="rId4" display="Tom16@way2automation.com" tooltip="mailto:Tom16@way2automation.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>